<commit_message>
update template laba rugi
</commit_message>
<xml_diff>
--- a/export/template/balance-sheet-template.xlsx
+++ b/export/template/balance-sheet-template.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr codeName="ThisWorkbook"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Backup SAYYID\#TRIPTA\triptatritunggal\export\template\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6780"/>
   </bookViews>
   <sheets>
-    <sheet name="Worksheet" sheetId="1" r:id="rId4"/>
+    <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1" forceFullCalc="1"/>
+  <calcPr calcId="162913" forceFullCalc="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="54">
   <si>
     <t>Balance Sheet Report ID</t>
   </si>
@@ -182,14 +186,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -216,13 +215,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -512,19 +519,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="9" max="9" width="13.28515625" customWidth="1"/>
+    <col min="14" max="14" width="21.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:27">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -607,7 +615,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:27">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -647,6 +655,9 @@
       <c r="M2">
         <v>1</v>
       </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
       <c r="O2" t="s">
         <v>35</v>
       </c>
@@ -659,7 +670,7 @@
       <c r="R2">
         <v>2</v>
       </c>
-      <c r="S2" t="b">
+      <c r="S2">
         <v>1</v>
       </c>
       <c r="T2" t="s">
@@ -687,7 +698,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:27">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -727,7 +738,7 @@
       <c r="M3">
         <v>1</v>
       </c>
-      <c r="N3" t="b">
+      <c r="N3">
         <v>1</v>
       </c>
       <c r="O3" t="s">
@@ -742,6 +753,9 @@
       <c r="R3">
         <v>2</v>
       </c>
+      <c r="S3">
+        <v>1</v>
+      </c>
       <c r="T3" t="s">
         <v>51</v>
       </c>
@@ -768,17 +782,6 @@
       </c>
     </row>
   </sheetData>
-  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
-  <tableParts count="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
enhance(BalanceSheetReport): update balance sheet
</commit_message>
<xml_diff>
--- a/export/template/balance-sheet-template.xlsx
+++ b/export/template/balance-sheet-template.xlsx
@@ -868,8 +868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L36" workbookViewId="0">
-      <selection activeCell="P47" sqref="P47"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -878,16 +878,16 @@
     <col min="2" max="2" width="3.42578125" customWidth="1"/>
     <col min="3" max="3" width="16.5703125" customWidth="1"/>
     <col min="4" max="4" width="25" customWidth="1"/>
-    <col min="5" max="5" width="26.7109375" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" customWidth="1"/>
-    <col min="7" max="7" width="25.140625" customWidth="1"/>
+    <col min="5" max="5" width="4.28515625" customWidth="1"/>
+    <col min="6" max="6" width="33.5703125" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" customWidth="1"/>
     <col min="8" max="8" width="14.85546875" customWidth="1"/>
     <col min="9" max="9" width="30" customWidth="1"/>
-    <col min="10" max="10" width="43.7109375" customWidth="1"/>
-    <col min="11" max="11" width="20.28515625" customWidth="1"/>
-    <col min="12" max="12" width="19.28515625" customWidth="1"/>
-    <col min="13" max="13" width="17.7109375" customWidth="1"/>
-    <col min="14" max="14" width="18.28515625" customWidth="1"/>
+    <col min="10" max="10" width="8.28515625" customWidth="1"/>
+    <col min="11" max="11" width="6.85546875" customWidth="1"/>
+    <col min="12" max="12" width="4.28515625" customWidth="1"/>
+    <col min="13" max="13" width="2.28515625" customWidth="1"/>
+    <col min="14" max="14" width="4" customWidth="1"/>
     <col min="15" max="15" width="45.5703125" customWidth="1"/>
     <col min="16" max="16" width="71.5703125" customWidth="1"/>
     <col min="17" max="17" width="17.85546875" customWidth="1"/>

</xml_diff>

<commit_message>
update database : update neraca , account ,account setting
</commit_message>
<xml_diff>
--- a/export/template/balance-sheet-template.xlsx
+++ b/export/template/balance-sheet-template.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="142">
   <si>
     <t>Balance Sheet Report ID</t>
   </si>
@@ -165,9 +165,6 @@
     <t>101.01.06</t>
   </si>
   <si>
-    <t>101.01.07</t>
-  </si>
-  <si>
     <t>101.01.08</t>
   </si>
   <si>
@@ -439,6 +436,15 @@
   </si>
   <si>
     <t>3#4#6#7#10#13#14#15#16#17#23#24#25#26#27#30#31#32#33#34#35#35#36#37#38#39#40#41#42#42#43#47</t>
+  </si>
+  <si>
+    <t>PPN Masukan</t>
+  </si>
+  <si>
+    <t>PPN Keluaran</t>
+  </si>
+  <si>
+    <t>JUMLAH HUTANG LANCAR</t>
   </si>
 </sst>
 </file>
@@ -868,8 +874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -878,8 +884,8 @@
     <col min="2" max="2" width="3.42578125" customWidth="1"/>
     <col min="3" max="3" width="16.5703125" customWidth="1"/>
     <col min="4" max="4" width="25" customWidth="1"/>
-    <col min="5" max="5" width="4.28515625" customWidth="1"/>
-    <col min="6" max="6" width="33.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" customWidth="1"/>
+    <col min="6" max="6" width="42.5703125" customWidth="1"/>
     <col min="7" max="7" width="11.5703125" customWidth="1"/>
     <col min="8" max="8" width="14.85546875" customWidth="1"/>
     <col min="9" max="9" width="30" customWidth="1"/>
@@ -1009,7 +1015,7 @@
         <v>200</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L2">
         <v>1</v>
@@ -1077,10 +1083,10 @@
         <v>15</v>
       </c>
       <c r="H3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L3">
         <v>3</v>
@@ -1148,10 +1154,10 @@
         <v>16</v>
       </c>
       <c r="H4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L4">
         <v>3</v>
@@ -1219,10 +1225,10 @@
         <v>17</v>
       </c>
       <c r="H5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L5">
         <v>3</v>
@@ -1290,10 +1296,10 @@
         <v>18</v>
       </c>
       <c r="H6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>55</v>
+        <v>140</v>
       </c>
       <c r="L6">
         <v>3</v>
@@ -1361,10 +1367,10 @@
         <v>19</v>
       </c>
       <c r="H7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="L7">
         <v>3</v>
@@ -1432,10 +1438,10 @@
         <v>20</v>
       </c>
       <c r="H8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="L8">
         <v>3</v>
@@ -1497,26 +1503,24 @@
         <v>47</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>35</v>
+        <v>139</v>
       </c>
       <c r="G9">
         <v>21</v>
       </c>
-      <c r="H9" s="12">
-        <v>0</v>
-      </c>
-      <c r="I9" s="2"/>
-      <c r="J9" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="K9" s="12" t="s">
-        <v>135</v>
-      </c>
+      <c r="H9" t="s">
+        <v>63</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
       <c r="L9">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="M9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N9">
         <v>1</v>
@@ -1568,11 +1572,11 @@
       <c r="D10">
         <v>9</v>
       </c>
-      <c r="E10" t="s">
-        <v>48</v>
+      <c r="E10">
+        <v>0</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -1580,8 +1584,17 @@
       <c r="H10">
         <v>0</v>
       </c>
+      <c r="I10" t="s">
+        <v>141</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="K10" s="12" t="s">
+        <v>134</v>
+      </c>
       <c r="L10">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="M10">
         <v>1</v>
@@ -1637,10 +1650,10 @@
         <v>10</v>
       </c>
       <c r="E11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G11">
         <v>23</v>
@@ -1649,7 +1662,7 @@
         <v>300</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L11">
         <v>3</v>
@@ -1708,10 +1721,10 @@
         <v>11</v>
       </c>
       <c r="E12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -1779,22 +1792,22 @@
         <v>0</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G13">
         <v>24</v>
       </c>
       <c r="H13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J13" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K13" s="12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L13">
         <v>6</v>
@@ -1855,20 +1868,20 @@
       <c r="E14">
         <v>0</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>40</v>
+      <c r="F14" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="G14">
         <v>25</v>
       </c>
       <c r="H14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J14" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L14">
         <v>6</v>
@@ -1929,14 +1942,17 @@
       <c r="E15">
         <v>0</v>
       </c>
+      <c r="F15" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="G15">
         <v>26</v>
       </c>
       <c r="H15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L15">
         <v>0</v>
@@ -1998,10 +2014,10 @@
         <v>27</v>
       </c>
       <c r="H16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="Q16">
         <v>10</v>
@@ -2057,10 +2073,10 @@
         <v>28</v>
       </c>
       <c r="H17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Q17">
         <v>10</v>
@@ -2116,10 +2132,10 @@
         <v>29</v>
       </c>
       <c r="H18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="Q18">
         <v>10</v>
@@ -2175,10 +2191,10 @@
         <v>30</v>
       </c>
       <c r="H19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q19">
         <v>0</v>
@@ -2234,10 +2250,10 @@
         <v>31</v>
       </c>
       <c r="H20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q20">
         <v>0</v>
@@ -2352,7 +2368,7 @@
         <v>400</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q22">
         <v>0</v>
@@ -2408,10 +2424,10 @@
         <v>33</v>
       </c>
       <c r="H23" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="Q23">
         <v>0</v>
@@ -2467,10 +2483,10 @@
         <v>34</v>
       </c>
       <c r="H24" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I24" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q24">
         <v>10</v>
@@ -2526,10 +2542,10 @@
         <v>35</v>
       </c>
       <c r="H25" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I25" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="Q25">
         <v>10</v>
@@ -2585,10 +2601,10 @@
         <v>36</v>
       </c>
       <c r="H26" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="Q26">
         <v>10</v>
@@ -2644,10 +2660,10 @@
         <v>37</v>
       </c>
       <c r="H27" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="Q27">
         <v>10</v>
@@ -2703,10 +2719,10 @@
         <v>38</v>
       </c>
       <c r="H28" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I28" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Q28">
         <v>10</v>
@@ -2818,10 +2834,10 @@
         <v>39</v>
       </c>
       <c r="H30" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I30" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="Q30">
         <v>0</v>
@@ -2877,10 +2893,10 @@
         <v>40</v>
       </c>
       <c r="H31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I31" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Q31">
         <v>10</v>
@@ -2936,10 +2952,10 @@
         <v>41</v>
       </c>
       <c r="H32" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I32" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Q32">
         <v>10</v>
@@ -2995,10 +3011,10 @@
         <v>42</v>
       </c>
       <c r="H33" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I33" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="Q33">
         <v>10</v>
@@ -3054,10 +3070,10 @@
         <v>43</v>
       </c>
       <c r="H34" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I34" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="Q34">
         <v>10</v>
@@ -3113,10 +3129,10 @@
         <v>44</v>
       </c>
       <c r="H35" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I35" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Q35">
         <v>10</v>
@@ -3172,10 +3188,10 @@
         <v>45</v>
       </c>
       <c r="H36" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I36" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="Q36">
         <v>10</v>
@@ -3231,10 +3247,10 @@
         <v>46</v>
       </c>
       <c r="H37" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I37" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="Q37">
         <v>10</v>
@@ -3290,10 +3306,10 @@
         <v>47</v>
       </c>
       <c r="H38" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I38" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="Q38">
         <v>10</v>
@@ -3349,10 +3365,10 @@
         <v>48</v>
       </c>
       <c r="H39" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I39" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="Q39">
         <v>10</v>
@@ -3408,10 +3424,10 @@
         <v>49</v>
       </c>
       <c r="H40" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I40" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q40">
         <v>10</v>
@@ -3467,10 +3483,10 @@
         <v>50</v>
       </c>
       <c r="H41" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I41" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Q41">
         <v>10</v>
@@ -3526,10 +3542,10 @@
         <v>51</v>
       </c>
       <c r="H42" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I42" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q42">
         <v>10</v>
@@ -3585,10 +3601,10 @@
         <v>52</v>
       </c>
       <c r="H43" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I43" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Q43">
         <v>10</v>
@@ -3644,10 +3660,10 @@
         <v>53</v>
       </c>
       <c r="H44" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I44" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Q44">
         <v>10</v>
@@ -3706,7 +3722,7 @@
         <v>0</v>
       </c>
       <c r="I45" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Q45">
         <v>0</v>
@@ -3762,10 +3778,10 @@
         <v>54</v>
       </c>
       <c r="H46" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Q46">
         <v>0</v>
@@ -3878,10 +3894,10 @@
         <v>55</v>
       </c>
       <c r="H48" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="Q48">
         <v>10</v>
@@ -3902,7 +3918,7 @@
         <v>1</v>
       </c>
       <c r="W48" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="X48">
         <v>0</v>
@@ -3994,16 +4010,16 @@
         <v>56</v>
       </c>
       <c r="H50" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I50" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="O50" s="12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="P50" s="12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q50">
         <v>11</v>
@@ -4118,7 +4134,7 @@
         <v>0</v>
       </c>
       <c r="I52" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q52" s="10">
         <v>0</v>

</xml_diff>

<commit_message>
enhance(Dev): update balance sheet report
</commit_message>
<xml_diff>
--- a/export/template/balance-sheet-template.xlsx
+++ b/export/template/balance-sheet-template.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="142">
   <si>
     <t>Balance Sheet Report ID</t>
   </si>
@@ -165,9 +165,6 @@
     <t>101.01.06</t>
   </si>
   <si>
-    <t>101.01.07</t>
-  </si>
-  <si>
     <t>101.01.08</t>
   </si>
   <si>
@@ -439,6 +436,15 @@
   </si>
   <si>
     <t>3#4#6#7#10#13#14#15#16#17#23#24#25#26#27#30#31#32#33#34#35#35#36#37#38#39#40#41#42#42#43#47</t>
+  </si>
+  <si>
+    <t>PPN Masukan</t>
+  </si>
+  <si>
+    <t>PPN Keluaran</t>
+  </si>
+  <si>
+    <t>JUMLAH HUTANG LANCAR</t>
   </si>
 </sst>
 </file>
@@ -868,8 +874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -878,8 +884,8 @@
     <col min="2" max="2" width="3.42578125" customWidth="1"/>
     <col min="3" max="3" width="16.5703125" customWidth="1"/>
     <col min="4" max="4" width="25" customWidth="1"/>
-    <col min="5" max="5" width="4.28515625" customWidth="1"/>
-    <col min="6" max="6" width="33.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" customWidth="1"/>
+    <col min="6" max="6" width="42.5703125" customWidth="1"/>
     <col min="7" max="7" width="11.5703125" customWidth="1"/>
     <col min="8" max="8" width="14.85546875" customWidth="1"/>
     <col min="9" max="9" width="30" customWidth="1"/>
@@ -1009,7 +1015,7 @@
         <v>200</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L2">
         <v>1</v>
@@ -1077,10 +1083,10 @@
         <v>15</v>
       </c>
       <c r="H3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L3">
         <v>3</v>
@@ -1148,10 +1154,10 @@
         <v>16</v>
       </c>
       <c r="H4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L4">
         <v>3</v>
@@ -1219,10 +1225,10 @@
         <v>17</v>
       </c>
       <c r="H5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L5">
         <v>3</v>
@@ -1290,10 +1296,10 @@
         <v>18</v>
       </c>
       <c r="H6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>55</v>
+        <v>140</v>
       </c>
       <c r="L6">
         <v>3</v>
@@ -1361,10 +1367,10 @@
         <v>19</v>
       </c>
       <c r="H7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="L7">
         <v>3</v>
@@ -1432,10 +1438,10 @@
         <v>20</v>
       </c>
       <c r="H8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="L8">
         <v>3</v>
@@ -1497,26 +1503,24 @@
         <v>47</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>35</v>
+        <v>139</v>
       </c>
       <c r="G9">
         <v>21</v>
       </c>
-      <c r="H9" s="12">
-        <v>0</v>
-      </c>
-      <c r="I9" s="2"/>
-      <c r="J9" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="K9" s="12" t="s">
-        <v>135</v>
-      </c>
+      <c r="H9" t="s">
+        <v>63</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
       <c r="L9">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="M9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N9">
         <v>1</v>
@@ -1568,11 +1572,11 @@
       <c r="D10">
         <v>9</v>
       </c>
-      <c r="E10" t="s">
-        <v>48</v>
+      <c r="E10">
+        <v>0</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -1580,8 +1584,17 @@
       <c r="H10">
         <v>0</v>
       </c>
+      <c r="I10" t="s">
+        <v>141</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="K10" s="12" t="s">
+        <v>134</v>
+      </c>
       <c r="L10">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="M10">
         <v>1</v>
@@ -1637,10 +1650,10 @@
         <v>10</v>
       </c>
       <c r="E11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G11">
         <v>23</v>
@@ -1649,7 +1662,7 @@
         <v>300</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L11">
         <v>3</v>
@@ -1708,10 +1721,10 @@
         <v>11</v>
       </c>
       <c r="E12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -1779,22 +1792,22 @@
         <v>0</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G13">
         <v>24</v>
       </c>
       <c r="H13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J13" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K13" s="12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L13">
         <v>6</v>
@@ -1855,20 +1868,20 @@
       <c r="E14">
         <v>0</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>40</v>
+      <c r="F14" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="G14">
         <v>25</v>
       </c>
       <c r="H14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J14" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L14">
         <v>6</v>
@@ -1929,14 +1942,17 @@
       <c r="E15">
         <v>0</v>
       </c>
+      <c r="F15" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="G15">
         <v>26</v>
       </c>
       <c r="H15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L15">
         <v>0</v>
@@ -1998,10 +2014,10 @@
         <v>27</v>
       </c>
       <c r="H16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="Q16">
         <v>10</v>
@@ -2057,10 +2073,10 @@
         <v>28</v>
       </c>
       <c r="H17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Q17">
         <v>10</v>
@@ -2116,10 +2132,10 @@
         <v>29</v>
       </c>
       <c r="H18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="Q18">
         <v>10</v>
@@ -2175,10 +2191,10 @@
         <v>30</v>
       </c>
       <c r="H19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q19">
         <v>0</v>
@@ -2234,10 +2250,10 @@
         <v>31</v>
       </c>
       <c r="H20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q20">
         <v>0</v>
@@ -2352,7 +2368,7 @@
         <v>400</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q22">
         <v>0</v>
@@ -2408,10 +2424,10 @@
         <v>33</v>
       </c>
       <c r="H23" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="Q23">
         <v>0</v>
@@ -2467,10 +2483,10 @@
         <v>34</v>
       </c>
       <c r="H24" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I24" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q24">
         <v>10</v>
@@ -2526,10 +2542,10 @@
         <v>35</v>
       </c>
       <c r="H25" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I25" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="Q25">
         <v>10</v>
@@ -2585,10 +2601,10 @@
         <v>36</v>
       </c>
       <c r="H26" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="Q26">
         <v>10</v>
@@ -2644,10 +2660,10 @@
         <v>37</v>
       </c>
       <c r="H27" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="Q27">
         <v>10</v>
@@ -2703,10 +2719,10 @@
         <v>38</v>
       </c>
       <c r="H28" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I28" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Q28">
         <v>10</v>
@@ -2818,10 +2834,10 @@
         <v>39</v>
       </c>
       <c r="H30" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I30" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="Q30">
         <v>0</v>
@@ -2877,10 +2893,10 @@
         <v>40</v>
       </c>
       <c r="H31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I31" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Q31">
         <v>10</v>
@@ -2936,10 +2952,10 @@
         <v>41</v>
       </c>
       <c r="H32" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I32" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Q32">
         <v>10</v>
@@ -2995,10 +3011,10 @@
         <v>42</v>
       </c>
       <c r="H33" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I33" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="Q33">
         <v>10</v>
@@ -3054,10 +3070,10 @@
         <v>43</v>
       </c>
       <c r="H34" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I34" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="Q34">
         <v>10</v>
@@ -3113,10 +3129,10 @@
         <v>44</v>
       </c>
       <c r="H35" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I35" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Q35">
         <v>10</v>
@@ -3172,10 +3188,10 @@
         <v>45</v>
       </c>
       <c r="H36" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I36" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="Q36">
         <v>10</v>
@@ -3231,10 +3247,10 @@
         <v>46</v>
       </c>
       <c r="H37" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I37" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="Q37">
         <v>10</v>
@@ -3290,10 +3306,10 @@
         <v>47</v>
       </c>
       <c r="H38" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I38" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="Q38">
         <v>10</v>
@@ -3349,10 +3365,10 @@
         <v>48</v>
       </c>
       <c r="H39" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I39" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="Q39">
         <v>10</v>
@@ -3408,10 +3424,10 @@
         <v>49</v>
       </c>
       <c r="H40" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I40" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q40">
         <v>10</v>
@@ -3467,10 +3483,10 @@
         <v>50</v>
       </c>
       <c r="H41" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I41" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Q41">
         <v>10</v>
@@ -3526,10 +3542,10 @@
         <v>51</v>
       </c>
       <c r="H42" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I42" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q42">
         <v>10</v>
@@ -3585,10 +3601,10 @@
         <v>52</v>
       </c>
       <c r="H43" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I43" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Q43">
         <v>10</v>
@@ -3644,10 +3660,10 @@
         <v>53</v>
       </c>
       <c r="H44" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I44" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Q44">
         <v>10</v>
@@ -3706,7 +3722,7 @@
         <v>0</v>
       </c>
       <c r="I45" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Q45">
         <v>0</v>
@@ -3762,10 +3778,10 @@
         <v>54</v>
       </c>
       <c r="H46" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Q46">
         <v>0</v>
@@ -3878,10 +3894,10 @@
         <v>55</v>
       </c>
       <c r="H48" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="Q48">
         <v>10</v>
@@ -3902,7 +3918,7 @@
         <v>1</v>
       </c>
       <c r="W48" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="X48">
         <v>0</v>
@@ -3994,16 +4010,16 @@
         <v>56</v>
       </c>
       <c r="H50" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I50" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="O50" s="12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="P50" s="12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q50">
         <v>11</v>
@@ -4118,7 +4134,7 @@
         <v>0</v>
       </c>
       <c r="I52" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q52" s="10">
         <v>0</v>

</xml_diff>